<commit_message>
not sure I changed anything (maybe just clicked save whan opening and closing the file) and git doesn't show differences
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Users\015004 ( Andrinopoulou )\Courses\Using R for Statistics in Medical Research (BST02)\BST02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Teaching\BST02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,6 +487,7 @@
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Slides: part A and B
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Teaching\BST02\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Users\015004 ( Andrinopoulou )\Courses\Using R for Statistics in Medical Research (BST02)\BST02\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Slides and demos Basic Use R
Slides and demos Basic Use R
mytemplate: added some packages for tables
gitignore: added the html files that are created for the demos , added the tex files for the slides, added the firuge folders
Schedule: added indexing in day 1
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Introduction</t>
   </si>
@@ -119,10 +119,10 @@
     <t>Practical</t>
   </si>
   <si>
-    <t>Tutorial</t>
-  </si>
-  <si>
     <t>Combination</t>
+  </si>
+  <si>
+    <t>Indexing</t>
   </si>
 </sst>
 </file>
@@ -476,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +554,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2">
         <v>1</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2">
         <v>1</v>
@@ -570,7 +570,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -578,7 +578,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D13" s="2">
         <v>1</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2">
         <v>1</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2">
         <v>1</v>
@@ -610,26 +610,26 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1</v>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D19" s="3">
         <v>2</v>
@@ -637,45 +637,45 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D20" s="3">
         <v>2</v>
       </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="3">
-        <v>2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D22" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="2">
-        <v>3</v>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D25" s="3">
         <v>4</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26" s="3">
         <v>4</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D27" s="3">
         <v>4</v>
@@ -699,36 +699,28 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D28" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="3">
-        <v>4</v>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>23</v>
-      </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D31" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D32" s="2">
         <v>5</v>
       </c>
     </row>

</xml_diff>